<commit_message>
improved testing and added tests
</commit_message>
<xml_diff>
--- a/test/xls/test.xlsx
+++ b/test/xls/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>url</t>
   </si>
@@ -91,6 +91,9 @@
   <si>
     <t>null</t>
   </si>
+  <si>
+    <t>send http get request</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -120,13 +123,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -177,7 +173,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -187,10 +183,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,18 +203,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -242,14 +233,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="313.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -260,6 +251,25 @@
       </c>
       <c r="F2" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added testing of the http response, both for the whole response and for regex match
</commit_message>
<xml_diff>
--- a/test/xls/test.xlsx
+++ b/test/xls/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>url</t>
   </si>
@@ -94,6 +94,24 @@
   <si>
     <t>send http get request</t>
   </si>
+  <si>
+    <t>expected response</t>
+  </si>
+  <si>
+    <t>expected response regex</t>
+  </si>
+  <si>
+    <t>http://requestb.in/re7qq8re</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>{"query":"data"}</t>
+  </si>
+  <si>
+    <t>o.</t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,6 +146,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -173,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +209,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -203,17 +232,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.4744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.24489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,6 +302,37 @@
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ability to send custom headers
</commit_message>
<xml_diff>
--- a/test/xls/test.xlsx
+++ b/test/xls/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>url</t>
   </si>
@@ -101,7 +101,10 @@
     <t>expected response regex</t>
   </si>
   <si>
-    <t>http://requestb.in/re7qq8re</t>
+    <t>headers</t>
+  </si>
+  <si>
+    <t>http://requestb.in/1jv3zq61</t>
   </si>
   <si>
     <t>ok</t>
@@ -111,6 +114,9 @@
   </si>
   <si>
     <t>o.</t>
+  </si>
+  <si>
+    <t>User-Agent=testx;Something='else entirely'</t>
   </si>
 </sst>
 </file>
@@ -234,18 +240,18 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F5:F6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.4744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.24489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.8826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,22 +323,28 @@
       <c r="E5" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check for expected response headers - issue #2
</commit_message>
<xml_diff>
--- a/test/xls/test.xlsx
+++ b/test/xls/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,30 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>json</t>
-  </si>
-  <si>
-    <t>$.hits.total</t>
-  </si>
-  <si>
-    <t>expected status code</t>
-  </si>
-  <si>
-    <t>$.hits.max_score</t>
-  </si>
-  <si>
-    <t>send http post request</t>
-  </si>
-  <si>
-    <t>graylog_0/_search</t>
-  </si>
-  <si>
-    <t>{
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$.hits.total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected status code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$.hits.max_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">send http post request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graylog_0/_search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
   "from": 0,
   "size": 150,
   "query": {
@@ -89,34 +89,40 @@
 }</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>send http get request</t>
-  </si>
-  <si>
-    <t>expected response</t>
-  </si>
-  <si>
-    <t>expected response regex</t>
-  </si>
-  <si>
-    <t>headers</t>
-  </si>
-  <si>
-    <t>http://requestb.in/1jv3zq61</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>{"query":"data"}</t>
-  </si>
-  <si>
-    <t>o.</t>
-  </si>
-  <si>
-    <t>User-Agent=testx;Something='else entirely'</t>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">send http get request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected response regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">headers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected headers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://requestb.in/12g5qd31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"query":"data"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User-Agent=testx;Something='else entirely'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content-type='text/html; charset=utf-8';'transfer-encoding'='chunked'</t>
   </si>
 </sst>
 </file>
@@ -124,9 +130,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,6 +166,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -218,6 +229,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,20 +253,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5:F6"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.8826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.12755102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,28 +343,37 @@
       <c r="F5" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="G5" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="http://requestb.in/12g5qd31"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>